<commit_message>
Added voltage divider to the humidity sensor. Redesigned layout
</commit_message>
<xml_diff>
--- a/OpenHAS_SensorBoard_v1.0/OpenHAS_SensorBoard_v1.0.xlsx
+++ b/OpenHAS_SensorBoard_v1.0/OpenHAS_SensorBoard_v1.0.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/balazsgollner/Documents/eagle/HomeAutomation_SensorBoard_v1.0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/balazsgollner/Documents/Projects/OpenHAS/Hardware/OpenHAS_SensorBoard_v1.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="32960" windowHeight="19000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="HomeAutomation_SensorBoard_v1.0" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="77">
   <si>
     <t>Qty</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>PROD_ID</t>
-  </si>
-  <si>
     <t>M02POLAR</t>
   </si>
   <si>
@@ -68,12 +65,6 @@
     <t>Resistor</t>
   </si>
   <si>
-    <t>10k</t>
-  </si>
-  <si>
-    <t>R7</t>
-  </si>
-  <si>
     <t>1uF</t>
   </si>
   <si>
@@ -146,9 +137,6 @@
     <t>Analog-output temperature sensor</t>
   </si>
   <si>
-    <t>IC-08917</t>
-  </si>
-  <si>
     <t>N-MOSFET</t>
   </si>
   <si>
@@ -161,9 +149,6 @@
     <t>Common NMOSFET Parts</t>
   </si>
   <si>
-    <t>TRAN-12988</t>
-  </si>
-  <si>
     <t>ON</t>
   </si>
   <si>
@@ -188,18 +173,12 @@
     <t>XBEE-2B3</t>
   </si>
   <si>
-    <t>XBEE-SMD</t>
-  </si>
-  <si>
     <t>XBEE1</t>
   </si>
   <si>
     <t>Xbee module footprints</t>
   </si>
   <si>
-    <t>CONN-09042</t>
-  </si>
-  <si>
     <t>0805</t>
   </si>
   <si>
@@ -209,39 +188,18 @@
     <t>Link</t>
   </si>
   <si>
-    <t>Price(HUF)</t>
-  </si>
-  <si>
     <t>2mm pitch, 10 pin receptacle</t>
   </si>
   <si>
     <t>Xbee socket</t>
   </si>
   <si>
-    <t>Sparkfun</t>
-  </si>
-  <si>
-    <t>https://www.sparkfun.com/products/10030</t>
-  </si>
-  <si>
-    <t>Price for a module</t>
-  </si>
-  <si>
-    <t>Total price per module</t>
-  </si>
-  <si>
-    <t>MacroBP</t>
-  </si>
-  <si>
     <t>Mouser</t>
   </si>
   <si>
     <t>http://hu.mouser.com/ProductDetail/Vishay-Semiconductors/TEMT6000X01/?qs=%2Fjqivxn91ccZGXDwz0wGxg%3D%3D</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>http://hu.mouser.com/ProductDetail/OSRAM-Opto-Semiconductors/LG-R971-KN-1/?qs=sGAEpiMZZMvyj6n1w4pZD2FClMF0hTzecNd8BzQWnaA%3d</t>
   </si>
   <si>
@@ -263,25 +221,56 @@
     <t>http://hu.mouser.com/ProductDetail/TE-Connectivity/1546215-2/?qs=sGAEpiMZZMvZTcaMAxB2AI%252bwpTxbJbcRsw7UMjeswrg%3d</t>
   </si>
   <si>
-    <t>Mouser part number</t>
-  </si>
-  <si>
-    <t>571-1546215-2</t>
-  </si>
-  <si>
-    <t>77-VJ0805A8R2BXQCBC</t>
+    <t>http://eu.mouser.com/ProductDetail/Vishay-Dale/CRCW0805100RFKEA/?qs=sGAEpiMZZMvdGkrng054txEw7b1YnvGuUG%2fFwliasrw%3d</t>
+  </si>
+  <si>
+    <t>5k</t>
+  </si>
+  <si>
+    <t>http://eu.mouser.com/ProductDetail/Vishay-Dale/CRCW08055K00FKTA/?qs=sGAEpiMZZMvdGkrng054t%2f1OkVvb3%2fZXh39j8BOI0pc%3d</t>
+  </si>
+  <si>
+    <t>http://eu.mouser.com/ProductDetail/AVX/F921A105MPA/?qs=sGAEpiMZZMuEN2agSAc2puC4lhRhLeolQ3t6vikRQaw%3d</t>
+  </si>
+  <si>
+    <t>R5, R7</t>
+  </si>
+  <si>
+    <t>4,7k</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>http://eu.mouser.com/ProductDetail/Yageo/RC0805FR-074K7L/?qs=sGAEpiMZZMvdGkrng054t8Tx25L%252bvTaR8bqsX3F4gtg%3d</t>
+  </si>
+  <si>
+    <t>http://eu.mouser.com/ProductDetail/Vishay-Dale/CRCW080564K9FKEA/?qs=sGAEpiMZZMvdGkrng054txEw7b1YnvGuw1wKTcry088%3d</t>
+  </si>
+  <si>
+    <t>http://eu.mouser.com/ProductDetail/Harwin/M22-7131042/?qs=sGAEpiMZZMs%252bGHln7q6pmzlZUuX%2f53qjCP17iTlpuwk%3d</t>
+  </si>
+  <si>
+    <t>http://eu.mouser.com/ProductDetail/Digi-International/XB24-Z7WIT-004/?qs=%2fha2pyFadugUPNrm22F93bP9LcVqSo9UynSGkDbK9pRABLav3eYkOL5AWCtHV%252bgu7nGpcUAl0ZQyZXJP%2fghRVsRsIQt8rsCkvXeOlbnRwQE%3d</t>
+  </si>
+  <si>
+    <t>XBEE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="42" formatCode="_-* #,##0\ &quot;HUF&quot;_-;\-* #,##0\ &quot;HUF&quot;_-;_-* &quot;-&quot;\ &quot;HUF&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;HUF&quot;_-;\-* #,##0.00\ &quot;HUF&quot;_-;_-* &quot;-&quot;??\ &quot;HUF&quot;_-;_-@_-"/>
-  </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -312,11 +301,11 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -594,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -607,84 +596,58 @@
     <col min="4" max="4" width="13.5" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>59</v>
-      </c>
-      <c r="I1" t="s">
-        <v>60</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="K1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
-        <v>10</v>
+      <c r="G2" t="s">
+        <v>56</v>
       </c>
       <c r="H2" t="s">
-        <v>69</v>
-      </c>
-      <c r="I2" t="s">
-        <v>78</v>
-      </c>
-      <c r="J2" s="3">
-        <v>147</v>
-      </c>
-      <c r="K2" s="3">
-        <f>A2*J2</f>
-        <v>147</v>
-      </c>
-      <c r="L2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -692,415 +655,360 @@
         <v>100</v>
       </c>
       <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3">
-        <f t="shared" ref="K3:K15" si="0">A3*J3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C6" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" t="s">
         <v>15</v>
       </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="F6" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s">
+      <c r="G6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" t="s">
         <v>18</v>
       </c>
-      <c r="F5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E7" t="s">
-        <v>23</v>
-      </c>
       <c r="F7" t="s">
-        <v>19</v>
+        <v>12</v>
+      </c>
+      <c r="G7" t="s">
+        <v>56</v>
       </c>
       <c r="H7" t="s">
-        <v>69</v>
-      </c>
-      <c r="I7" t="s">
-        <v>77</v>
-      </c>
-      <c r="J7" s="3">
-        <v>15</v>
-      </c>
-      <c r="K7" s="3">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="L7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>31</v>
+        <v>16</v>
+      </c>
+      <c r="G8" t="s">
+        <v>56</v>
       </c>
       <c r="H8" t="s">
-        <v>69</v>
-      </c>
-      <c r="I8" t="s">
-        <v>76</v>
-      </c>
-      <c r="J8" s="3">
-        <v>2150</v>
-      </c>
-      <c r="K8" s="3">
-        <f t="shared" si="0"/>
-        <v>2150</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F9" t="s">
-        <v>35</v>
+        <v>28</v>
+      </c>
+      <c r="G9" t="s">
+        <v>56</v>
       </c>
       <c r="H9" t="s">
-        <v>69</v>
-      </c>
-      <c r="I9" t="s">
-        <v>75</v>
-      </c>
-      <c r="J9" s="3">
-        <v>152</v>
-      </c>
-      <c r="K9" s="3">
-        <f t="shared" si="0"/>
-        <v>152</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="F10" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="G10" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="H10" t="s">
-        <v>69</v>
-      </c>
-      <c r="I10" t="s">
-        <v>74</v>
-      </c>
-      <c r="J10" s="3">
-        <v>87.81</v>
-      </c>
-      <c r="K10" s="3">
-        <f t="shared" si="0"/>
-        <v>87.81</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
       <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" t="s">
+        <v>56</v>
+      </c>
+      <c r="H11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" t="s">
+        <v>56</v>
+      </c>
+      <c r="H12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
         <v>41</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" t="s">
-        <v>44</v>
-      </c>
-      <c r="G11" t="s">
-        <v>45</v>
-      </c>
-      <c r="H11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I11" t="s">
-        <v>73</v>
-      </c>
-      <c r="J11" s="3">
-        <v>75</v>
-      </c>
-      <c r="K11" s="3">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>2</v>
-      </c>
-      <c r="B12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F12" t="s">
-        <v>26</v>
-      </c>
-      <c r="H12" t="s">
-        <v>69</v>
-      </c>
-      <c r="I12" t="s">
-        <v>72</v>
-      </c>
-      <c r="J12" s="3">
-        <v>16.25</v>
-      </c>
-      <c r="K12" s="3">
-        <f t="shared" si="0"/>
-        <v>32.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E13" t="s">
-        <v>51</v>
-      </c>
       <c r="F13" t="s">
-        <v>52</v>
+        <v>23</v>
+      </c>
+      <c r="G13" t="s">
+        <v>56</v>
       </c>
       <c r="H13" t="s">
-        <v>69</v>
-      </c>
-      <c r="I13" t="s">
-        <v>70</v>
-      </c>
-      <c r="J13" s="3">
-        <v>236.86</v>
-      </c>
-      <c r="K13" s="3">
-        <f t="shared" si="0"/>
-        <v>236.86</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" t="s">
+        <v>56</v>
+      </c>
+      <c r="H14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" t="s">
+        <v>56</v>
+      </c>
+      <c r="H15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" t="s">
         <v>54</v>
       </c>
-      <c r="E14" t="s">
-        <v>55</v>
-      </c>
-      <c r="F14" t="s">
-        <v>56</v>
-      </c>
-      <c r="G14" t="s">
-        <v>57</v>
-      </c>
-      <c r="H14" t="s">
-        <v>68</v>
-      </c>
-      <c r="I14" t="s">
-        <v>71</v>
-      </c>
-      <c r="J14" s="2">
-        <v>8840</v>
-      </c>
-      <c r="K14" s="3">
-        <f t="shared" si="0"/>
-        <v>8840</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>2</v>
-      </c>
-      <c r="B15" t="s">
-        <v>63</v>
-      </c>
-      <c r="C15" t="s">
-        <v>62</v>
-      </c>
-      <c r="F15" t="s">
-        <v>62</v>
-      </c>
-      <c r="H15" t="s">
-        <v>64</v>
-      </c>
-      <c r="I15" t="s">
-        <v>65</v>
-      </c>
-      <c r="J15" s="3">
-        <v>265.32</v>
-      </c>
-      <c r="K15" s="3">
-        <f t="shared" si="0"/>
-        <v>530.64</v>
-      </c>
-    </row>
-    <row r="21" spans="9:11" x14ac:dyDescent="0.2">
-      <c r="I21" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="J21" s="4"/>
-      <c r="K21" s="3">
-        <f>SUM(K2:K20)</f>
-        <v>12266.81</v>
-      </c>
+      <c r="F16" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16" t="s">
+        <v>56</v>
+      </c>
+      <c r="H16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H22" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="I21:J21"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>